<commit_message>
14-01-2019 : clients update changes
</commit_message>
<xml_diff>
--- a/database/finance_management.xlsx
+++ b/database/finance_management.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>system manages all financial transactions in form of receivable incomes.</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>display yearly income with a graphical view.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module Description </t>
+  </si>
+  <si>
+    <t>Srno</t>
   </si>
 </sst>
 </file>
@@ -84,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,8 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,90 +401,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>